<commit_message>
Finish testing hallucination checker
</commit_message>
<xml_diff>
--- a/out/hallucination_report.xlsx
+++ b/out/hallucination_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,19 +467,6 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>24EM03358</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>PDF not found or exam number incorrect</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update color of figures and implement N° prélèvement checker
</commit_message>
<xml_diff>
--- a/out/hallucination_report.xlsx
+++ b/out/hallucination_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>sample</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>status</t>
         </is>
       </c>
@@ -461,9 +466,28 @@
           <t>chr5:1295228C&gt;T (C228T)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Mutation not found in PDF or ambiguity</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>24EM03462</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>24219576 1.1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N° de prélèvement not found in PDF or ambiguity</t>
         </is>
       </c>
     </row>

</xml_diff>